<commit_message>
Add unit tests for dataUploadService
</commit_message>
<xml_diff>
--- a/src/test/resources/data_sample.xlsx
+++ b/src/test/resources/data_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rvenant/DEVELOPPEMENT/COURANT/UNPIUT/ExplorateurIUT/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DB5DF3-68B1-4B41-88EC-53469D24C245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4580917F-64B2-F34A-9DF1-F9275AFC42B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8020" yWindow="880" windowWidth="30240" windowHeight="17680" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IUT" sheetId="1" r:id="rId1"/>
@@ -516,59 +516,59 @@
     <t xml:space="preserve">Publicité </t>
   </si>
   <si>
-    <t>emplacement</t>
-  </si>
-  <si>
-    <t>titres/Objets</t>
-  </si>
-  <si>
-    <t>corps texte 1</t>
-  </si>
-  <si>
-    <t>corps texte 2</t>
-  </si>
-  <si>
-    <t>corps texte 3</t>
-  </si>
-  <si>
-    <t>corps texte 4</t>
-  </si>
-  <si>
-    <t>url 1</t>
-  </si>
-  <si>
-    <t>url2</t>
-  </si>
-  <si>
-    <t>page accueil</t>
-  </si>
-  <si>
-    <t>fiche pratique1</t>
-  </si>
-  <si>
-    <t>fiche pratique2</t>
-  </si>
-  <si>
-    <t>fiche pratique3</t>
-  </si>
-  <si>
-    <t>fiche pratique4</t>
-  </si>
-  <si>
-    <t>Mails groupés</t>
-  </si>
-  <si>
     <t>GRAND-EST</t>
   </si>
   <si>
     <t>Commentaires (Hors BD)</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>contenu</t>
+  </si>
+  <si>
+    <t>accueilTitre</t>
+  </si>
+  <si>
+    <t>Bienvenue sur ExplorerIUT</t>
+  </si>
+  <si>
+    <t>accueilSousTitre</t>
+  </si>
+  <si>
+    <t>vous accompagne pour faciliter votre recherche de futurs apprentis</t>
+  </si>
+  <si>
+    <t>accueilTitreRecherche</t>
+  </si>
+  <si>
+    <t>Une recherche simple et rapide en 3 étapes</t>
+  </si>
+  <si>
+    <t>case1Titre</t>
+  </si>
+  <si>
+    <t>1 – Recherchez les formations qui vous intéressent</t>
+  </si>
+  <si>
+    <t>case1Texte</t>
+  </si>
+  <si>
+    <t>Avec visualisation des contenus et des débouchés de chaque formation</t>
+  </si>
+  <si>
+    <t>case2Titre</t>
+  </si>
+  <si>
+    <t>2 – Localisez les IUT qui vous intéressent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -649,8 +649,19 @@
       <color rgb="FF000000"/>
       <name val="Söhne"/>
     </font>
+    <font>
+      <b/>
+      <sz val="7.5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7.5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -673,6 +684,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
   </fills>
@@ -881,7 +898,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1017,6 +1034,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1444,7 +1467,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1455,7 +1478,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>9</v>
@@ -1545,7 +1568,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>28</v>
@@ -1691,7 +1714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2229,7 +2252,7 @@
       <c r="AC13" s="24"/>
       <c r="AD13" s="24"/>
     </row>
-    <row r="14" spans="1:30" ht="208">
+    <row r="14" spans="1:30" ht="192">
       <c r="A14" s="15" t="s">
         <v>48</v>
       </c>
@@ -2549,7 +2572,7 @@
       <c r="AC21" s="24"/>
       <c r="AD21" s="24"/>
     </row>
-    <row r="22" spans="1:30" ht="272">
+    <row r="22" spans="1:30" ht="288">
       <c r="A22" s="15" t="s">
         <v>45</v>
       </c>
@@ -9535,74 +9558,74 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="50.5" customWidth="1"/>
     <col min="4" max="4" width="51.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B1" s="52" t="s">
         <v>138</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="3" spans="1:2" ht="24">
+      <c r="A3" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B3" s="53" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="53" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
+      <c r="B4" s="53" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" ht="24">
+      <c r="A5" s="53" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
+      <c r="B5" s="53" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" ht="24">
+      <c r="A6" s="53" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
+      <c r="B6" s="53" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="53" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Polish and lot of changes
</commit_message>
<xml_diff>
--- a/src/test/resources/data_sample.xlsx
+++ b/src/test/resources/data_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rvenant/DEVELOPPEMENT/COURANT/UNPIUT/ExplorateurIUT/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4580917F-64B2-F34A-9DF1-F9275AFC42B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FDFCE2-A466-454E-9B7C-B137FD399B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8020" yWindow="880" windowWidth="30240" windowHeight="17680" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -651,12 +651,12 @@
     </font>
     <font>
       <b/>
-      <sz val="7.5"/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="7.5"/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1718,7 +1718,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15"/>
@@ -9560,19 +9560,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.5" customWidth="1"/>
     <col min="4" max="4" width="51.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="17">
       <c r="A1" s="52" t="s">
         <v>137</v>
       </c>
@@ -9580,7 +9580,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="17">
       <c r="A2" s="53" t="s">
         <v>139</v>
       </c>
@@ -9588,7 +9588,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="24">
+    <row r="3" spans="1:2" ht="34">
       <c r="A3" s="53" t="s">
         <v>141</v>
       </c>
@@ -9596,7 +9596,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="34">
       <c r="A4" s="53" t="s">
         <v>143</v>
       </c>
@@ -9604,7 +9604,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="24">
+    <row r="5" spans="1:2" ht="34">
       <c r="A5" s="53" t="s">
         <v>145</v>
       </c>
@@ -9612,7 +9612,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="24">
+    <row r="6" spans="1:2" ht="34">
       <c r="A6" s="53" t="s">
         <v>147</v>
       </c>
@@ -9620,7 +9620,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" ht="17">
       <c r="A7" s="53" t="s">
         <v>149</v>
       </c>

</xml_diff>

<commit_message>
Externalize backend mail text components into the Excel data file
</commit_message>
<xml_diff>
--- a/src/test/resources/data_sample.xlsx
+++ b/src/test/resources/data_sample.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rvenant/DEVELOPPEMENT/COURANT/UNPIUT/ExplorateurIUT/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FDFCE2-A466-454E-9B7C-B137FD399B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1ED8941-EE20-6A43-8CE6-66287D51D894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8020" yWindow="880" windowWidth="30240" windowHeight="17680" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8020" yWindow="880" windowWidth="30240" windowHeight="17680" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IUT" sheetId="1" r:id="rId1"/>
     <sheet name="BUT" sheetId="2" r:id="rId2"/>
     <sheet name="TEXTES" sheetId="3" r:id="rId3"/>
+    <sheet name="TEXTES_COURIELS" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="177">
   <si>
     <t>IUT</t>
   </si>
@@ -563,12 +564,90 @@
   <si>
     <t>2 – Localisez les IUT qui vous intéressent</t>
   </si>
+  <si>
+    <t>courielIUT_enteteBonjour</t>
+  </si>
+  <si>
+    <t>Bonjour ceci est un mail automatique de Exploriut,</t>
+  </si>
+  <si>
+    <t>courielIUT_deptConcernesLabel</t>
+  </si>
+  <si>
+    <t>Les départements concernés par ce mail sont :</t>
+  </si>
+  <si>
+    <t>courielIUT_pieceJointeAttentionLabel</t>
+  </si>
+  <si>
+    <t>Attention, les possibles offres en pièces jointes peuvent être destinées à d'autres départements.</t>
+  </si>
+  <si>
+    <t>courielIUT_demandeTransmission</t>
+  </si>
+  <si>
+    <t>Merci de transmettre cette demande au service compétent au sein de votre IUT et dans l’attente d’un retour rapide,</t>
+  </si>
+  <si>
+    <t>courielIUT_identiteLabel</t>
+  </si>
+  <si>
+    <t>Identité :</t>
+  </si>
+  <si>
+    <t>courielIUT_entrepriseLabel</t>
+  </si>
+  <si>
+    <t>Nom entreprise :</t>
+  </si>
+  <si>
+    <t>courielIUT_fonctionLabel</t>
+  </si>
+  <si>
+    <t>Fonction dans l'entreprise :</t>
+  </si>
+  <si>
+    <t>courielIUT_mailContactLabel</t>
+  </si>
+  <si>
+    <t>Mail du contact :</t>
+  </si>
+  <si>
+    <t>courielConfirmation_sujet</t>
+  </si>
+  <si>
+    <t>ExplorIUT - Confirmation de la recherche d'alternance</t>
+  </si>
+  <si>
+    <t>courielConfirmation_enteteBonjour</t>
+  </si>
+  <si>
+    <t>Bonjour</t>
+  </si>
+  <si>
+    <t>courielConfirmation_textePrincipal</t>
+  </si>
+  <si>
+    <t>Suite à votre demande de contact avec les IUT de France, vous devez confirmer votre envoi en cliquant sur ce lien :</t>
+  </si>
+  <si>
+    <t>courielConfirmation_formulePolitesse</t>
+  </si>
+  <si>
+    <t>Cordialement,</t>
+  </si>
+  <si>
+    <t>courielConfirmation_signature</t>
+  </si>
+  <si>
+    <t>ExplorIUT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -660,8 +739,28 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -690,6 +789,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
   </fills>
@@ -898,7 +1003,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1041,6 +1146,11 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -9560,7 +9670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -9632,4 +9742,135 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F047FF-607A-7749-B140-3AB9BB5C70BB}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16">
+      <c r="A1" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="55" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="55" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="55" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="56" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="56" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" s="56" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="56" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>